<commit_message>
Added Validations to Test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Drybar/DrybarTestData.xlsx
+++ b/src/test/resources/TestData/Drybar/DrybarTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varap\playwright-java-framework\src\test\resources\TestData\Drybar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B08782-A415-495E-8A9D-121E188D6788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6C8BE0-AB93-49A9-A088-F989B4B25F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>